<commit_message>
add provider location script and csv; update Rmd for  scripts, Exported_Data
</commit_message>
<xml_diff>
--- a/External Data/reports/2014_termination_data.xlsx
+++ b/External Data/reports/2014_termination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TedSc\OneDrive\Desktop\R Projects\20221214_IN_ab_gest\IN_ab_gest\External_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TedSc\OneDrive\Desktop\R Projects\indiana_abortion\External Data\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29D526B-CEEB-4417-8491-1052B8043F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBBE986C-1B12-408D-8CDF-5B9D99518E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="821" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="695" yWindow="695" windowWidth="17480" windowHeight="9930" tabRatio="821" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2014_age" sheetId="1" r:id="rId1"/>
@@ -529,10 +529,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Planned Parenthood of Indiana and Kentucky - Indianapolis
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Planned Parenthood of Indiana and Kentucky - Lafayette
 </t>
   </si>
@@ -560,6 +556,9 @@
   </si>
   <si>
     <t>Dilation Evacuation</t>
+  </si>
+  <si>
+    <t>Planned Parenthood of Indiana and Kentucky– Indianapolis</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1058,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1423,12 +1422,12 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" s="7" t="s">
         <v>154</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1460,7 @@
         <v>3.31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1471,7 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -1483,7 +1482,7 @@
         <v>33.229999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>26.66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>16.149999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -1516,7 +1515,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -1538,7 +1537,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
@@ -1555,9 +1554,9 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -1617,7 +1616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>129</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -1737,7 +1736,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1757,7 +1756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -1797,7 +1796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>114</v>
       </c>
@@ -1817,7 +1816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -1857,7 +1856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -1877,7 +1876,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -1897,7 +1896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1917,7 +1916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2077,7 +2076,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2157,7 +2156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -2190,12 +2189,12 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>58.36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>28.66</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2239,7 +2238,7 @@
         <v>3.12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>7.48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2294,7 +2293,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
@@ -2310,12 +2309,12 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2337,7 +2336,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>91.23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
@@ -2375,13 +2374,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="27.6328125" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>8.51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2436,7 +2435,7 @@
         <v>20.28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>15.21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v>12.47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2469,7 +2468,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2480,7 +2479,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="6"/>
     </row>
   </sheetData>
@@ -2504,83 +2503,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="24.90625" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="9"/>
+    <col min="3" max="3" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2">
         <v>27</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0.33259423503325941</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1">
         <v>2165</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>26.669130327666913</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>5926</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>72.998275437299824</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
@@ -2593,186 +2592,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="53.54296875" customWidth="1"/>
-    <col min="2" max="2" width="34.36328125" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="9"/>
+    <col min="2" max="2" width="34.36328125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>159</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C2">
         <v>32</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>0.3942343230257484</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C3">
         <v>998</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>12.295182949365529</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C4">
         <v>158</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>1.9465319699396328</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="1">
         <v>1179</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>14.52507083897992</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>2973</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>36.62683257361094</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C7">
         <v>718</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>8.8456326228902302</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="C8">
         <v>169</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>2.0820500184797339</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1">
         <v>1070</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>13.182210176173465</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C10">
         <v>788</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>9.7080202045090545</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
         <v>160</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>4.927929037821855E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C12">
         <v>28</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0.34495503264752986</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
@@ -2788,14 +2787,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="15.08984375" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2809,7 +2808,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.75">
       <c r="C18" s="4"/>
     </row>
   </sheetData>
@@ -2867,13 +2866,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="18.1796875" style="7" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>78.819999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" s="7" t="s">
         <v>151</v>
       </c>
@@ -2906,7 +2905,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" s="7" t="s">
         <v>59</v>
       </c>
@@ -2917,7 +2916,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" s="7" t="s">
         <v>57</v>
       </c>
@@ -2952,31 +2951,31 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="8.1796875" style="7" customWidth="1"/>
     <col min="2" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" t="s">
         <v>164</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>166</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>4238</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="7" t="s">
         <v>153</v>
       </c>
@@ -3004,7 +3003,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="7" t="s">
         <v>59</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="7" t="s">
         <v>57</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="F8" s="5"/>
       <c r="H8" s="3"/>
     </row>

</xml_diff>

<commit_message>
add monthly data to reports; add script to clean monthly data and script to visualize; add monthly visualizations and datatable to dashboard; update precise provider map to import  prov_ll.csv  rather than geocode addresses in Rmd; update Readme files.
</commit_message>
<xml_diff>
--- a/External Data/reports/2014_termination_data.xlsx
+++ b/External Data/reports/2014_termination_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TedSc\OneDrive\Desktop\R Projects\indiana_abortion\External Data\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBBE986C-1B12-408D-8CDF-5B9D99518E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95E4980-1A9C-4E6D-897A-F8227580137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="695" yWindow="695" windowWidth="17480" windowHeight="9930" tabRatio="821" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="1315" windowWidth="16490" windowHeight="9485" tabRatio="821" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2014_age" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="2014_gestation" sheetId="8" r:id="rId8"/>
     <sheet name="2014_gestation_procedure" sheetId="9" r:id="rId9"/>
     <sheet name="2014_county" sheetId="10" r:id="rId10"/>
+    <sheet name="2014_monthly" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="186">
   <si>
     <t>15-17</t>
   </si>
@@ -559,6 +560,51 @@
   </si>
   <si>
     <t>Planned Parenthood of Indiana and Kentucky– Indianapolis</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Resident Terminations_x000D_(n = 7621)</t>
+  </si>
+  <si>
+    <t>Non-Resident Terminations_x000D_(n = 497)</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1093,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1059,7 +1105,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -2181,6 +2226,164 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A012CB0F-44A4-457C-84FE-5855389EDB9E}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2">
+        <v>687</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3">
+        <v>657</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4">
+        <v>732</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5">
+        <v>666</v>
+      </c>
+      <c r="C5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6">
+        <v>704</v>
+      </c>
+      <c r="C6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7">
+        <v>609</v>
+      </c>
+      <c r="C7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8">
+        <v>599</v>
+      </c>
+      <c r="C8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9">
+        <v>654</v>
+      </c>
+      <c r="C9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10">
+        <v>553</v>
+      </c>
+      <c r="C10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11">
+        <v>650</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12">
+        <v>535</v>
+      </c>
+      <c r="C12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13">
+        <v>575</v>
+      </c>
+      <c r="C13">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
@@ -2592,14 +2795,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="53.54296875" customWidth="1"/>
-    <col min="2" max="2" width="34.36328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="34.36328125" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
@@ -2607,7 +2810,7 @@
       <c r="A1" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>54</v>
       </c>
       <c r="C1" t="s">
@@ -2621,7 +2824,7 @@
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" t="s">
         <v>52</v>
       </c>
       <c r="C2">
@@ -2635,7 +2838,7 @@
       <c r="A3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" t="s">
         <v>50</v>
       </c>
       <c r="C3">
@@ -2649,7 +2852,7 @@
       <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" t="s">
         <v>48</v>
       </c>
       <c r="C4">
@@ -2663,7 +2866,7 @@
       <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="1">
@@ -2677,7 +2880,7 @@
       <c r="A6" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="1">
@@ -2691,7 +2894,7 @@
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" t="s">
         <v>44</v>
       </c>
       <c r="C7">
@@ -2705,7 +2908,7 @@
       <c r="A8" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" t="s">
         <v>43</v>
       </c>
       <c r="C8">
@@ -2719,7 +2922,7 @@
       <c r="A9" t="s">
         <v>162</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="1">
@@ -2733,7 +2936,7 @@
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
       <c r="C10">
@@ -2747,7 +2950,7 @@
       <c r="A11" t="s">
         <v>160</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
       <c r="C11">
@@ -2761,7 +2964,7 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" t="s">
         <v>37</v>
       </c>
       <c r="C12">

</xml_diff>